<commit_message>
Retouche des maquettes et documentation dans la documentation technique + journal de bord
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\TPI2020\docs\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11596A5F-7782-4319-9871-350AAF50D9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3240EAA9-3363-4C86-8418-0A64D5C1B85E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -878,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AC7D34-5216-48CF-9639-7D59B4738AE5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -2100,68 +2100,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="13" width="11.5703125" customWidth="1"/>
+    <col min="2" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="27">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -2169,20 +2167,21 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="18">
-        <f>SUM(C2:M2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L2" s="17"/>
+      <c r="M2" s="18">
+        <f>SUM(B2:L2)</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="27">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2190,20 +2189,19 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="18">
-        <f t="shared" ref="N3:N45" si="0">SUM(C3:M3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="7"/>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3:M45" si="0">SUM(B3:L3)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -2211,20 +2209,19 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" s="7"/>
+      <c r="M4" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -2232,20 +2229,21 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" s="7"/>
+      <c r="M5" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="27">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -2253,20 +2251,19 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L6" s="7"/>
+      <c r="M6" s="18">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -2274,20 +2271,19 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="7"/>
+      <c r="M7" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2295,20 +2291,19 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="7"/>
+      <c r="M8" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2316,20 +2311,19 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L9" s="7"/>
+      <c r="M9" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2337,20 +2331,19 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" s="7"/>
+      <c r="M10" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2358,20 +2351,19 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="7"/>
+      <c r="M11" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2379,20 +2371,19 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="7"/>
+      <c r="M12" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -2400,20 +2391,19 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L13" s="7"/>
+      <c r="M13" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2421,20 +2411,19 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="7"/>
+      <c r="M14" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -2442,18 +2431,17 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="7"/>
+      <c r="M15" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2463,18 +2451,17 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" s="7"/>
+      <c r="M16" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2484,18 +2471,17 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="7"/>
+      <c r="M17" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2505,18 +2491,17 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="7"/>
+      <c r="M18" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2526,18 +2511,17 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="7"/>
+      <c r="M19" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2547,18 +2531,17 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="7"/>
+      <c r="M20" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2568,18 +2551,17 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="7"/>
+      <c r="M21" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2589,18 +2571,17 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="7"/>
+      <c r="M22" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2610,18 +2591,17 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="7"/>
+      <c r="M23" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2631,18 +2611,17 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="7"/>
+      <c r="M24" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -2652,18 +2631,17 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L25" s="7"/>
+      <c r="M25" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="26"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2673,18 +2651,17 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L26" s="7"/>
+      <c r="M26" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2694,18 +2671,17 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L27" s="7"/>
+      <c r="M27" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2715,18 +2691,17 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L28" s="7"/>
+      <c r="M28" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="26"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2736,18 +2711,17 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L29" s="7"/>
+      <c r="M29" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="26"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -2757,18 +2731,17 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L30" s="7"/>
+      <c r="M30" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="26"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2778,20 +2751,19 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="7"/>
+      <c r="M31" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2799,19 +2771,18 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L32" s="7"/>
+      <c r="M32" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2820,18 +2791,17 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="7"/>
+      <c r="M33" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="26"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -2841,18 +2811,17 @@
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="24"/>
+      <c r="M34" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -2862,18 +2831,17 @@
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="24"/>
+      <c r="M35" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="26"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -2883,18 +2851,17 @@
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L36" s="24"/>
+      <c r="M36" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="26"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -2904,18 +2871,17 @@
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L37" s="24"/>
+      <c r="M37" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="26"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
@@ -2925,18 +2891,17 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L38" s="24"/>
+      <c r="M38" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="26"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
@@ -2946,18 +2911,17 @@
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L39" s="24"/>
+      <c r="M39" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="26"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -2967,18 +2931,17 @@
       <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L40" s="24"/>
+      <c r="M40" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="26"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
@@ -2988,18 +2951,17 @@
       <c r="I41" s="18"/>
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L41" s="24"/>
+      <c r="M41" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="26"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -3009,18 +2971,19 @@
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L42" s="24"/>
+      <c r="M42" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="26"/>
+      <c r="B43" s="27">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
@@ -3030,18 +2993,17 @@
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
       <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L43" s="24"/>
+      <c r="M43" s="18">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="26"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
@@ -3051,18 +3013,17 @@
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
       <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L44" s="24"/>
+      <c r="M44" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -3072,16 +3033,15 @@
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
       <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L45" s="24"/>
+      <c r="M45" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="28"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
@@ -3091,14 +3051,13 @@
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
       <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="18"/>
-    </row>
-    <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L46" s="24"/>
+      <c r="M46" s="18"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
       <c r="F47" s="30"/>
@@ -3107,17 +3066,16 @@
       <c r="I47" s="30"/>
       <c r="J47" s="30"/>
       <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="18"/>
-    </row>
-    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="31"/>
+      <c r="M47" s="18"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="31">
-        <f t="shared" ref="B48:L48" si="1">SUM(B2:B45)</f>
-        <v>0</v>
+        <f t="shared" ref="B48:K48" si="1">SUM(B2:B45)</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C48" s="31">
         <f t="shared" si="1"/>
@@ -3156,16 +3114,12 @@
         <v>0</v>
       </c>
       <c r="L48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="31">
-        <f>SUM(M2:M45)</f>
-        <v>0</v>
-      </c>
-      <c r="N48" s="18"/>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+        <f>SUM(L2:L45)</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="18"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -3176,18 +3130,17 @@
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
       <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
+      <c r="L49" s="18">
+        <f>SUM(B48:L48)</f>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="M49" s="18">
-        <f>SUM(C48:M48)</f>
-        <v>0</v>
-      </c>
-      <c r="N49" s="18">
-        <f>SUM(N2:N45)</f>
-        <v>0</v>
+        <f>SUM(M2:M45)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:M45">
+  <conditionalFormatting sqref="B2:L45">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Modification des maquettes et de la base de données + documentation de la modification
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3240EAA9-3363-4C86-8418-0A64D5C1B85E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCCE517-3664-441A-8BE9-529D3E9C4850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Planification</t>
   </si>
   <si>
-    <t>Importation des données de test</t>
-  </si>
-  <si>
     <t>Page d'accueil</t>
   </si>
   <si>
@@ -102,12 +99,6 @@
     <t>Contrôleurs</t>
   </si>
   <si>
-    <t>Menu dynamique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestion des droits </t>
-  </si>
-  <si>
     <t>Doc technique</t>
   </si>
   <si>
@@ -141,72 +132,15 @@
     <t>Implémentation de la base de données</t>
   </si>
   <si>
-    <t>table User (CRUD)</t>
-  </si>
-  <si>
-    <t>table Course (CRUD)</t>
-  </si>
-  <si>
-    <t>table Role (read.. Pas forcément utile)</t>
-  </si>
-  <si>
-    <t>Page login/logout + email</t>
-  </si>
-  <si>
-    <t>Page ajout cours</t>
-  </si>
-  <si>
-    <t>Page modification cours</t>
-  </si>
-  <si>
-    <t>Page inscription à un cours</t>
-  </si>
-  <si>
-    <t>Page reservation utilisateur</t>
-  </si>
-  <si>
-    <t>Accueil (liste des cours)</t>
-  </si>
-  <si>
-    <t>Cours (horaire, nombre de places)</t>
-  </si>
-  <si>
-    <t>Edition Cours</t>
-  </si>
-  <si>
-    <t>Inscription Cours</t>
-  </si>
-  <si>
     <t>Gestion Admin</t>
   </si>
   <si>
-    <t>Pages administrateurs</t>
-  </si>
-  <si>
     <t>Maquettage</t>
   </si>
   <si>
-    <t>table Reservations (CRUD)</t>
-  </si>
-  <si>
-    <t>table Tokens (CRUD)</t>
-  </si>
-  <si>
-    <t>Table Preferences (CRUD)</t>
-  </si>
-  <si>
-    <t>Classe Esession</t>
-  </si>
-  <si>
-    <t>Utilisateurs (cours inscrit + nombre inscrpition possible)</t>
-  </si>
-  <si>
     <t>Envoi emails</t>
   </si>
   <si>
-    <t>Ajax</t>
-  </si>
-  <si>
     <t>Page login</t>
   </si>
   <si>
@@ -262,6 +196,12 @@
   </si>
   <si>
     <t>Suppression film</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Connexion BD</t>
   </si>
 </sst>
 </file>
@@ -465,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -536,6 +476,27 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,7 +840,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +946,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="26">
         <v>8.3333333333333329E-2</v>
@@ -1010,7 +971,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1035,7 +996,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6" s="26">
         <v>0.125</v>
@@ -1060,7 +1021,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18"/>
@@ -1081,7 +1042,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1106,7 +1067,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="26">
         <v>4.1666666666666664E-2</v>
@@ -1131,7 +1092,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B10" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1156,7 +1117,7 @@
     </row>
     <row r="11" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B11" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1181,7 +1142,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B12" s="26">
         <v>4.1666666666666664E-2</v>
@@ -1206,7 +1167,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B13" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1231,7 +1192,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B14" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1256,7 +1217,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B15" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1281,7 +1242,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B16" s="26">
         <v>4.1666666666666664E-2</v>
@@ -1303,7 +1264,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="1"/>
@@ -1324,7 +1285,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1349,7 +1310,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B19" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1374,7 +1335,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B20" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1399,7 +1360,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B21" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1424,7 +1385,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="1"/>
@@ -1445,7 +1406,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B23" s="26">
         <v>6.25E-2</v>
@@ -1470,7 +1431,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B24" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1495,7 +1456,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B25" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1517,7 +1478,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="26">
         <v>2.0833333333333332E-2</v>
@@ -1542,7 +1503,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B27" s="26">
         <v>8.3333333333333329E-2</v>
@@ -1567,7 +1528,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B28" s="26">
         <v>0.125</v>
@@ -1596,7 +1557,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B29" s="26">
         <v>0.16666666666666666</v>
@@ -1625,7 +1586,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B30" s="26">
         <v>4.1666666666666664E-2</v>
@@ -1650,7 +1611,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B31" s="26">
         <v>0.16666666666666666</v>
@@ -1679,7 +1640,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B32" s="26">
         <v>8.3333333333333329E-2</v>
@@ -1706,7 +1667,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B33" s="26">
         <v>8.3333333333333329E-2</v>
@@ -1733,7 +1694,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B34" s="26">
         <v>8.3333333333333329E-2</v>
@@ -1757,7 +1718,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B35" s="26">
         <v>0.14583333333333334</v>
@@ -1779,7 +1740,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="18"/>
@@ -1800,7 +1761,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" s="26">
         <v>0.33333333333333331</v>
@@ -1829,7 +1790,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" s="26">
         <v>0.25</v>
@@ -1879,7 +1840,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B40" s="26">
         <v>0.91666666666666663</v>
@@ -1924,7 +1885,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B41" s="26">
         <v>0.33333333333333331</v>
@@ -1959,7 +1920,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B42" s="26">
         <v>8.3333333333333329E-2</v>
@@ -2100,7 +2061,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2152,10 +2113,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C2" s="18"/>
@@ -2174,10 +2135,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="18">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C3" s="18"/>
@@ -2191,16 +2152,18 @@
       <c r="K3" s="1"/>
       <c r="L3" s="7"/>
       <c r="M3" s="18">
-        <f t="shared" ref="M3:M45" si="0">SUM(B3:L3)</f>
+        <f t="shared" ref="M3:M40" si="0">SUM(B3:L3)</f>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2212,15 +2175,17 @@
       <c r="L4" s="7"/>
       <c r="M4" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="18"/>
+      <c r="A5" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2232,14 +2197,14 @@
       <c r="L5" s="7"/>
       <c r="M5" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="27">
+      <c r="A6" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="18">
         <v>0.14583333333333334</v>
       </c>
       <c r="C6" s="18"/>
@@ -2258,10 +2223,10 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="27"/>
+      <c r="A7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="18"/>
       <c r="C7" s="18"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2278,10 +2243,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="27"/>
+      <c r="A8" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="18"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2298,10 +2263,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="27"/>
+      <c r="A9" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2318,10 +2283,10 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="27"/>
+      <c r="A10" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2337,11 +2302,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="27"/>
+    <row r="11" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2358,10 +2323,10 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="27"/>
+      <c r="A12" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2377,11 +2342,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="27"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2398,10 +2363,10 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="27"/>
+      <c r="A14" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2418,10 +2383,10 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="27"/>
+      <c r="A15" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2438,10 +2403,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="27"/>
+      <c r="A16" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="18"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2452,16 +2417,13 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="27"/>
+      <c r="A17" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="18"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2478,10 +2440,10 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="27"/>
+      <c r="A18" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="18"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2498,11 +2460,13 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2514,14 +2478,14 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="27"/>
+      <c r="A20" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="18"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2538,10 +2502,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="27"/>
+      <c r="A21" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="18"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2550,7 +2514,6 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
       <c r="L21" s="7"/>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
@@ -2558,10 +2521,10 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="27"/>
+      <c r="A22" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="18"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2570,7 +2533,6 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
       <c r="L22" s="7"/>
       <c r="M22" s="18">
         <f t="shared" si="0"/>
@@ -2578,10 +2540,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="27"/>
+      <c r="A23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="18"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2592,16 +2554,13 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="7"/>
-      <c r="M23" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="27"/>
+      <c r="A24" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="18"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2618,10 +2577,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="27"/>
+      <c r="A25" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="18"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -2638,11 +2597,11 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2658,10 +2617,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="27"/>
+      <c r="A27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="18"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2678,130 +2637,124 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="7"/>
+      <c r="A28" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="24"/>
       <c r="M28" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="7"/>
+      <c r="A29" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="24"/>
       <c r="M29" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="7"/>
+      <c r="A30" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="24"/>
       <c r="M30" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="7"/>
+      <c r="A31" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="24"/>
       <c r="M31" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="27"/>
+      <c r="A32" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="18"/>
       <c r="C32" s="18"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A33" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="27"/>
+      <c r="A34" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -2818,10 +2771,10 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="27"/>
+      <c r="A35" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -2838,10 +2791,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="27"/>
+      <c r="A36" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -2858,10 +2811,10 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="27"/>
+      <c r="A37" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
@@ -2878,11 +2831,15 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C38" s="18">
+        <v>0.125</v>
+      </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -2891,17 +2848,17 @@
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="24"/>
+      <c r="L38" s="18"/>
       <c r="M38" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(B38:L38)</f>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="27"/>
+      <c r="A39" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="18"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
@@ -2918,10 +2875,10 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="27"/>
+      <c r="A40" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
@@ -2938,10 +2895,8 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="27"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
@@ -2952,58 +2907,75 @@
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
       <c r="L41" s="24"/>
-      <c r="M41" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="27">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="18">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="M41" s="18"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="23"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="18"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="31">
+        <f t="shared" ref="B43:L43" si="1">SUM(B2:B40)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C43" s="31">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="18"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="27"/>
+      <c r="B44" s="18"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
@@ -3013,134 +2985,11 @@
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
       <c r="K44" s="18"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="18"/>
-    </row>
-    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="18"/>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="31">
-        <f t="shared" ref="B48:K48" si="1">SUM(B2:B45)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K48" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L48" s="31">
-        <f>SUM(L2:L45)</f>
-        <v>0</v>
-      </c>
-      <c r="M48" s="18"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18">
-        <f>SUM(B48:L48)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="M49" s="18">
-        <f>SUM(M2:M45)</f>
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:L45">
+  <conditionalFormatting sqref="B40:L40 C23:L39 C21:J22 L21:L22 C2:L20 B26 B28:B39 B2:B24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
correction des maquettes et de la bdd + documentation dans doc technique
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCCE517-3664-441A-8BE9-529D3E9C4850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD282D3F-935D-469C-84BC-B1BF2E718B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="7" r:id="rId1"/>
@@ -839,9 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AC7D34-5216-48CF-9639-7D59B4738AE5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2063,7 +2061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2186,7 +2184,9 @@
       <c r="C5" s="18">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -2197,7 +2197,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="18">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,9 @@
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2456,7 +2458,7 @@
       <c r="L18" s="7"/>
       <c r="M18" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2467,7 +2469,9 @@
       <c r="C19" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2478,7 +2482,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.22916666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2840,7 +2844,9 @@
       <c r="C38" s="18">
         <v>0.125</v>
       </c>
-      <c r="D38" s="18"/>
+      <c r="D38" s="18">
+        <v>0.125</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
@@ -2851,7 +2857,7 @@
       <c r="L38" s="18"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.20833333333333331</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2938,7 +2944,7 @@
       </c>
       <c r="D43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="E43" s="31">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
création des méthodes + documentation
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD282D3F-935D-469C-84BC-B1BF2E718B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A694EA-ADA1-49D3-8FE6-37371D1319C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="7" r:id="rId1"/>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AC7D34-5216-48CF-9639-7D59B4738AE5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2061,7 +2061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2187,7 +2187,9 @@
       <c r="D5" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -2197,7 +2199,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="18">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2207,9 +2209,13 @@
       <c r="B6" s="18">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -2219,7 +2225,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="18">
         <f t="shared" si="0"/>
-        <v>0.14583333333333334</v>
+        <v>0.18750000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2472,7 +2478,9 @@
       <c r="D19" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2482,7 +2490,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>0.22916666666666669</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2842,22 +2850,24 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C38" s="18">
-        <v>0.125</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="D38" s="18">
         <v>0.125</v>
       </c>
-      <c r="E38" s="18"/>
+      <c r="E38" s="18">
+        <v>0.125</v>
+      </c>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
+      <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.33333333333333331</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2940,7 +2950,7 @@
       </c>
       <c r="C43" s="31">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D43" s="31">
         <f t="shared" si="1"/>
@@ -2948,7 +2958,7 @@
       </c>
       <c r="E43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="F43" s="31">
         <f t="shared" si="1"/>
@@ -2995,7 +3005,7 @@
       <c r="M44" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B40:L40 C23:L39 C21:J22 L21:L22 C2:L20 B26 B28:B39 B2:B24">
+  <conditionalFormatting sqref="B40:L40 C21:J22 L21:L22 C2:L20 B26 B28:B39 B2:B24 C23:L39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
inscription + login avec mail
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A694EA-ADA1-49D3-8FE6-37371D1319C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230F7B0B-1051-48E0-BAE5-6C7848B94C17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2276,7 +2276,9 @@
       <c r="C9" s="18"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2285,7 +2287,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2296,7 +2298,9 @@
       <c r="C10" s="18"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2305,7 +2309,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2316,7 +2320,9 @@
       <c r="C11" s="18"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -2325,7 +2331,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2481,7 +2487,9 @@
       <c r="E19" s="1">
         <v>0.14583333333333334</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2490,7 +2498,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2540,7 +2548,9 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2548,7 +2558,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2559,7 +2569,9 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2576,7 +2588,9 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2585,7 +2599,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2858,7 +2872,9 @@
       <c r="E38" s="18">
         <v>0.125</v>
       </c>
-      <c r="F38" s="18"/>
+      <c r="F38" s="18">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
@@ -2867,7 +2883,7 @@
       <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.4375</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2962,7 +2978,7 @@
       </c>
       <c r="F43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="G43" s="31">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
avancement du site + documentation
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230F7B0B-1051-48E0-BAE5-6C7848B94C17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F0CADE-89DC-4972-AE83-C46D8D1F412B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2256,7 +2256,9 @@
       <c r="C8" s="18"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2265,7 +2267,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2343,7 +2345,9 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2351,7 +2355,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2363,7 +2367,9 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2371,7 +2377,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2403,7 +2409,9 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2411,7 +2419,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2488,7 +2496,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="F19" s="1">
-        <v>0.10416666666666667</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2498,7 +2506,7 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>0.47916666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2529,7 +2537,9 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2537,7 +2547,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2611,7 +2621,9 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2619,7 +2631,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2631,7 +2643,9 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <v>6.25E-2</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2639,7 +2653,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2691,7 +2705,9 @@
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
@@ -2699,7 +2715,7 @@
       <c r="L29" s="24"/>
       <c r="M29" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2731,7 +2747,9 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="G31" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
@@ -2739,7 +2757,7 @@
       <c r="L31" s="24"/>
       <c r="M31" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2751,7 +2769,9 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="G32" s="18">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
@@ -2873,9 +2893,11 @@
         <v>0.125</v>
       </c>
       <c r="F38" s="18">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="G38" s="18"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G38" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
@@ -2883,7 +2905,7 @@
       <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.54166666666666663</v>
+        <v>0.60416666666666674</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2978,11 +3000,11 @@
       </c>
       <c r="F43" s="31">
         <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H43" s="31">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
filtre + gestion users + suppression films et blocage
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626DEB52-314F-44ED-ABB2-FCA79A4049B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC978F4-F7C4-4AA5-8AFF-4B930B9349FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="7" r:id="rId1"/>
@@ -2062,7 +2062,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,14 +2194,16 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="7"/>
       <c r="M5" s="18">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2288,14 +2290,16 @@
       <c r="G9" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="7"/>
       <c r="M9" s="18">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2398,14 +2402,16 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="7"/>
       <c r="M14" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2440,7 +2446,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2549,13 +2557,15 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="L21" s="7"/>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2674,14 +2684,16 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="7"/>
       <c r="M27" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2694,14 +2706,16 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
+      <c r="H28" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
       <c r="L28" s="24"/>
       <c r="M28" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2736,14 +2750,16 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
+      <c r="H30" s="18">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="L30" s="24"/>
       <c r="M30" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2758,14 +2774,16 @@
       <c r="G31" s="18">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H31" s="18"/>
+      <c r="H31" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
       <c r="L31" s="24"/>
       <c r="M31" s="18">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2906,14 +2924,16 @@
       <c r="G38" s="18">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H38" s="18"/>
+      <c r="H38" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
       <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.5625</v>
+        <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3016,7 +3036,7 @@
       </c>
       <c r="H43" s="31">
         <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I43" s="31">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
fin du huitieme jour
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC978F4-F7C4-4AA5-8AFF-4B930B9349FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F736795-BAEE-480F-952A-6A6AB177FC07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Connexion BD</t>
+  </si>
+  <si>
+    <t>Debuggage / peaufinage</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,10 +2252,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
@@ -2293,21 +2293,23 @@
       <c r="H9" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <v>6.25E-2</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="7"/>
       <c r="M9" s="18">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>36</v>
+      <c r="A10" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -2317,16 +2319,15 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
       <c r="L10" s="7"/>
       <c r="M10" s="18">
-        <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <f>SUM(B10:L10)</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -2346,9 +2347,9 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -2357,9 +2358,7 @@
       <c r="F12" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G12" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -2367,20 +2366,22 @@
       <c r="L12" s="7"/>
       <c r="M12" s="18">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G13" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2394,39 +2395,39 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="G14" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="7"/>
       <c r="M14" s="18">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2438,26 +2439,29 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="18"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="G16" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="18"/>
+      <c r="M16" s="18">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
-        <v>20</v>
+      <c r="A17" s="38" t="s">
+        <v>39</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="1"/>
@@ -2465,25 +2469,25 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="7"/>
       <c r="M17" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>56</v>
+      <c r="A18" s="37" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -2492,28 +2496,19 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="18">
-        <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="18"/>
-      <c r="C19" s="1">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.14583333333333334</v>
-      </c>
-      <c r="F19" s="1">
-        <v>6.25E-2</v>
-      </c>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2522,18 +2517,26 @@
       <c r="L19" s="7"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>0.4375</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
-        <v>21</v>
+      <c r="A20" s="39" t="s">
+        <v>55</v>
       </c>
       <c r="B20" s="18"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6.25E-2</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2542,35 +2545,32 @@
       <c r="L20" s="7"/>
       <c r="M20" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>43</v>
+      <c r="A21" s="40" t="s">
+        <v>21</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1">
-        <v>2.0833333333333332E-2</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
       <c r="L21" s="7"/>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="1"/>
@@ -2580,13 +2580,15 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="L22" s="7"/>
       <c r="M22" s="18">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2687,13 +2689,15 @@
       <c r="H27" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="7"/>
       <c r="M27" s="18">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2803,11 +2807,14 @@
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
       <c r="L32" s="24"/>
-      <c r="M32" s="18"/>
+      <c r="M32" s="18">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2816,11 +2823,16 @@
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="I33" s="18">
+        <v>0.125</v>
+      </c>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
       <c r="L33" s="24"/>
-      <c r="M33" s="18"/>
+      <c r="M33" s="18">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
@@ -2837,10 +2849,7 @@
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
       <c r="L34" s="24"/>
-      <c r="M34" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M34" s="18"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
@@ -2897,10 +2906,7 @@
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
       <c r="L37" s="24"/>
-      <c r="M37" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="M37" s="18"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
@@ -2927,13 +2933,15 @@
       <c r="H38" s="18">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I38" s="18"/>
+      <c r="I38" s="18">
+        <v>6.25E-2</v>
+      </c>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
       <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.64583333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3040,7 +3048,7 @@
       </c>
       <c r="I43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J43" s="31">
         <f t="shared" si="1"/>
@@ -3071,7 +3079,7 @@
       <c r="M44" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B40:L40 C21:J22 L21:L22 C2:L20 B26 B28:B39 B2:B24 C23:L39">
+  <conditionalFormatting sqref="B40:L40 C22:J22 C10:J10 L22 L10 C2:L9 C11:L21 B26 B28:B39 B2:B24 C23:L39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
affichage medias dynamiquement + manuel utilisateur
</commit_message>
<xml_diff>
--- a/docs/analysis/planification.xlsx
+++ b/docs/analysis/planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebRoot\EvaluationFilms\docs\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F736795-BAEE-480F-952A-6A6AB177FC07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC0ED3E-07C0-45AD-A89E-93C906FDC5E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Debuggage / peaufinage</t>
+  </si>
+  <si>
+    <t>Manuel utilisateur</t>
   </si>
 </sst>
 </file>
@@ -2064,9 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2826,12 +2827,14 @@
       <c r="I33" s="18">
         <v>0.125</v>
       </c>
-      <c r="J33" s="18"/>
+      <c r="J33" s="18">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="K33" s="18"/>
       <c r="L33" s="24"/>
       <c r="M33" s="18">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -2936,17 +2939,19 @@
       <c r="I38" s="18">
         <v>6.25E-2</v>
       </c>
-      <c r="J38" s="18"/>
+      <c r="J38" s="18">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="K38" s="18"/>
       <c r="L38" s="24"/>
       <c r="M38" s="18">
         <f>SUM(B38:L38)</f>
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -2956,12 +2961,14 @@
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
+      <c r="J39" s="18">
+        <v>0.125</v>
+      </c>
       <c r="K39" s="18"/>
       <c r="L39" s="24"/>
       <c r="M39" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3052,7 +3059,7 @@
       </c>
       <c r="J43" s="31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K43" s="31">
         <f t="shared" si="1"/>

</xml_diff>